<commit_message>
bug fix 3 string to int conversion
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17760" windowWidth="38400" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191028" calcMode="manual" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" calcMode="manual" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -64,28 +64,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -453,24 +453,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20.42578125"/>
-    <col customWidth="1" max="10" min="2" width="12.7109375"/>
+    <col width="20.44140625" customWidth="1" min="1" max="1"/>
+    <col width="12.6640625" customWidth="1" min="2" max="10"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="45.75" r="1" s="2">
+    <row r="1" ht="45.75" customFormat="1" customHeight="1" s="2">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Unique ID</t>
@@ -989,459 +989,100 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>207555731976</t>
-        </is>
+      <c r="A11" t="n">
+        <v>902634020041</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>19105006</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Shubham</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>8059241611</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>in</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>in</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>207555731976</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>19105077</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Shreyas</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>7589802655</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>in</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2279590476710</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>19105092</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Ashok</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>8968963929</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>19105092</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Ashok</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>8968963929</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>19105092</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Ashok</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>8968963929</t>
-        </is>
-      </c>
       <c r="K14" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>19105092</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Ashok</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>8968963929</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>19105092</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Ashok</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>8968963929</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>79590476710</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>781678351607</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>279590476710</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>19105092</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Ashok</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>8968963929</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>781678351607</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>781678351607</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>207555731976</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>19105077</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Shreyas</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>7589802655</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>902634020041</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>19105006</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Shubham</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>8059241611</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>902634020041</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>19105006</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Shubham</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>8059241611</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>in</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>781678351607</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Ansh</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
         <is>
           <t>in</t>
         </is>
@@ -1449,16 +1090,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H10" r:id="rId9"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H8" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
milestione 1 with no bugs
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12456" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" calcMode="manual" fullCalcOnLoad="1"/>
@@ -64,28 +64,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -453,7 +453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -466,11 +466,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20.44140625" customWidth="1" min="1" max="1"/>
-    <col width="12.6640625" customWidth="1" min="2" max="10"/>
+    <col customWidth="1" max="1" min="1" width="20.44140625"/>
+    <col customWidth="1" max="10" min="2" width="12.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45.75" customFormat="1" customHeight="1" s="2">
+    <row customFormat="1" customHeight="1" ht="45.75" r="1" s="2">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Unique ID</t>
@@ -1090,16 +1090,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
-    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H10" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>